<commit_message>
updated moscow docuent and interview questions
</commit_message>
<xml_diff>
--- a/Documentation/Information/Feature Analysis-MoSCoW-v17.xlsx
+++ b/Documentation/Information/Feature Analysis-MoSCoW-v17.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tafewa-my.sharepoint.com/personal/j162548_tafe_wa_edu_au/Documents/NFS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20069271\Documents\GitHub\NavyFoodSecurity\Documentation\Information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="263" documentId="11_2F05675EFD41A23E2A6F228FF25232F32934C093" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{090DDE3F-2707-4E4E-9AC1-8C4F741EC6CE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories (MoSCoW)" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'User Stories (MoSCoW)'!$A$1:$M$17</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'User Stories (MoSCoW)'!$1:$8</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -45,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="78">
   <si>
     <t>Project:</t>
   </si>
@@ -146,12 +145,6 @@
     <t>Acceptance Criteria</t>
   </si>
   <si>
-    <t>1.1</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
     <t>Must</t>
   </si>
   <si>
@@ -161,9 +154,6 @@
     <t>I can access my stored data</t>
   </si>
   <si>
-    <t>1.2</t>
-  </si>
-  <si>
     <t>Should</t>
   </si>
   <si>
@@ -173,66 +163,33 @@
     <t>My data is not open to another person without permission</t>
   </si>
   <si>
-    <t>1.3</t>
-  </si>
-  <si>
-    <t>update my profile</t>
-  </si>
-  <si>
-    <t>It is up to date, and accurate</t>
-  </si>
-  <si>
-    <t>1.4</t>
-  </si>
-  <si>
     <t>change my password</t>
   </si>
   <si>
     <t>I can keep my data secure</t>
   </si>
   <si>
-    <t>1.5</t>
-  </si>
-  <si>
     <t>recover my password</t>
   </si>
   <si>
     <t>when I have lost my password, I can reset it</t>
   </si>
   <si>
-    <t>1.6</t>
-  </si>
-  <si>
-    <t>Won't</t>
-  </si>
-  <si>
     <t>Browse Users</t>
   </si>
   <si>
-    <t>Information remains private?</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
     <t>Manage Users</t>
   </si>
   <si>
     <t>I can Manage Users</t>
   </si>
   <si>
-    <t>2.1</t>
-  </si>
-  <si>
     <t>Delete User</t>
   </si>
   <si>
     <t>Unauthorised personnel cannot access the system</t>
   </si>
   <si>
-    <t>2.2</t>
-  </si>
-  <si>
     <t>Edit User</t>
   </si>
   <si>
@@ -257,9 +214,6 @@
     <t>I can manage delivery locations</t>
   </si>
   <si>
-    <t>Delivery Manager</t>
-  </si>
-  <si>
     <t>Unauthorised Personnel cannot access sensitive GPS data</t>
   </si>
   <si>
@@ -303,12 +257,33 @@
   </si>
   <si>
     <t>You may need to do a little formatting clean-up. Best way is to highlight a row (eg 10), press the format painter button, then click in column A of the row you wish to cleanup.</t>
+  </si>
+  <si>
+    <t>Scan QR code</t>
+  </si>
+  <si>
+    <t>I can revreive order information</t>
+  </si>
+  <si>
+    <t>update my profile role</t>
+  </si>
+  <si>
+    <t>It is appropriate according to my current duty</t>
+  </si>
+  <si>
+    <t>General User</t>
+  </si>
+  <si>
+    <t>Create an order</t>
+  </si>
+  <si>
+    <t>An order can be placed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -757,7 +732,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -802,9 +777,6 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -962,36 +934,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="29" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="29" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1019,6 +961,36 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="29" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="29" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="30">
@@ -1056,160 +1028,6 @@
   <dxfs count="33">
     <dxf>
       <font>
-        <b/>
-        <i/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1481,6 +1299,160 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1584,7 +1556,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="NMT Table" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="NMT Table" pivot="0" count="6" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="NMT Table" pivot="0" count="6">
       <tableStyleElement type="wholeTable" dxfId="32"/>
       <tableStyleElement type="headerRow" dxfId="31"/>
       <tableStyleElement type="totalRow" dxfId="30"/>
@@ -1605,8 +1577,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A8:M31" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
-  <autoFilter ref="A8:M31" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:M31" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A8:M31">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1620,27 +1592,27 @@
     <filterColumn colId="12" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date Added" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ID" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="As A" dataDxfId="22">
+    <tableColumn id="1" name="Date Added" dataDxfId="12"/>
+    <tableColumn id="2" name="ID" dataDxfId="11"/>
+    <tableColumn id="3" name="As A" dataDxfId="10">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="User Type/Role" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="I" dataDxfId="20">
+    <tableColumn id="4" name="User Type/Role" dataDxfId="9"/>
+    <tableColumn id="5" name="I" dataDxfId="8">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="MoSCoW Priority" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="be able to" dataDxfId="18">
+    <tableColumn id="6" name="MoSCoW Priority" dataDxfId="7"/>
+    <tableColumn id="7" name="be able to" dataDxfId="6">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Feature Description" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="So That" dataDxfId="16">
+    <tableColumn id="8" name="Feature Description" dataDxfId="5"/>
+    <tableColumn id="9" name="So That" dataDxfId="4">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Business Reason" dataDxfId="15"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Version" dataDxfId="14"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Developer (s) Responsible" dataDxfId="13"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Acceptance Criteria" dataDxfId="12"/>
+    <tableColumn id="10" name="Business Reason" dataDxfId="3"/>
+    <tableColumn id="15" name="Version" dataDxfId="2"/>
+    <tableColumn id="14" name="Developer (s) Responsible" dataDxfId="1"/>
+    <tableColumn id="13" name="Acceptance Criteria" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="NMT Table" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1917,15 +1889,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="129" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="129" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13:XFD13"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1935,137 +1907,137 @@
     <col min="3" max="3" width="8.375" customWidth="1"/>
     <col min="4" max="4" width="18.875" customWidth="1"/>
     <col min="5" max="5" width="5" style="14" customWidth="1"/>
-    <col min="6" max="6" width="19.5" style="25" customWidth="1"/>
-    <col min="7" max="7" width="14.125" style="25" customWidth="1"/>
-    <col min="8" max="8" width="51.125" style="48" customWidth="1"/>
-    <col min="9" max="9" width="10.75" style="25" customWidth="1"/>
-    <col min="10" max="10" width="63" style="48" customWidth="1"/>
+    <col min="6" max="6" width="19.5" style="24" customWidth="1"/>
+    <col min="7" max="7" width="14.125" style="24" customWidth="1"/>
+    <col min="8" max="8" width="51.125" style="47" customWidth="1"/>
+    <col min="9" max="9" width="10.75" style="24" customWidth="1"/>
+    <col min="10" max="10" width="63" style="47" customWidth="1"/>
     <col min="11" max="11" width="11.75" customWidth="1"/>
     <col min="12" max="12" width="30" customWidth="1"/>
     <col min="13" max="13" width="62.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="73" t="s">
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="71" t="s">
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="72"/>
-      <c r="M1" s="75"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="84"/>
     </row>
     <row r="2" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="20" t="s">
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="20" t="s">
         <v>6</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="77" t="s">
+      <c r="L2" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="78"/>
+      <c r="M2" s="87"/>
     </row>
     <row r="3" spans="1:13" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="22" t="s">
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="24" t="s">
+      <c r="J3" s="23" t="s">
         <v>14</v>
       </c>
       <c r="K3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="76" t="s">
+      <c r="L3" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="79"/>
+      <c r="M3" s="88"/>
     </row>
     <row r="4" spans="1:13" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:13" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="86"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="82"/>
-      <c r="J5" s="82"/>
-      <c r="K5" s="87"/>
-      <c r="L5" s="88"/>
-      <c r="M5" s="89"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="71"/>
+      <c r="K5" s="76"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="78"/>
     </row>
     <row r="6" spans="1:13" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:13" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="83" t="s">
+      <c r="A7" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="84"/>
-      <c r="J7" s="84"/>
-      <c r="K7" s="80" t="s">
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="81"/>
+      <c r="L7" s="70"/>
       <c r="M7" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="32" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="15" t="s">
@@ -2086,792 +2058,700 @@
       <c r="G8" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="26" t="s">
+      <c r="H8" s="25" t="s">
         <v>27</v>
       </c>
       <c r="I8" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="27" t="s">
+      <c r="J8" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="K8" s="34" t="s">
+      <c r="K8" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="L8" s="35" t="s">
+      <c r="L8" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="M8" s="36" t="s">
+      <c r="M8" s="35" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="37">
-        <v>43843</v>
-      </c>
-      <c r="B9" s="55" t="s">
+    <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="36"/>
+      <c r="B9" s="54">
+        <v>1</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="16" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
-        <v>As A</v>
-      </c>
-      <c r="D9" s="10" t="s">
+      <c r="G9" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="16" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
-        <v>I</v>
-      </c>
-      <c r="F9" s="10" t="s">
+      <c r="I9" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="16" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
-        <v>be able to</v>
-      </c>
-      <c r="H9" s="28" t="s">
+      <c r="K9" s="38"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="39"/>
+    </row>
+    <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="40"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" s="38"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="39"/>
+    </row>
+    <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="40"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="K11" s="38"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="39"/>
+    </row>
+    <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="40"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" s="38"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="39"/>
+    </row>
+    <row r="13" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="40"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="16" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
-        <v>So That</v>
-      </c>
-      <c r="J9" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="K9" s="39"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="40"/>
+      <c r="G13" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="K13" s="38"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="39"/>
     </row>
-    <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="41">
-        <v>43843</v>
-      </c>
-      <c r="B10" s="56" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="17" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
-        <v>As A</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="17" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
-        <v>I</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="17" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
-        <v>be able to</v>
-      </c>
-      <c r="H10" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" s="17" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
-        <v>So That</v>
-      </c>
-      <c r="J10" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="K10" s="39"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="40"/>
+    <row r="14" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="40"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="K14" s="38"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="39"/>
     </row>
-    <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="41">
-        <v>43843</v>
-      </c>
-      <c r="B11" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="17" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
-        <v>As A</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="17" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
-        <v>I</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="17" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
-        <v>be able to</v>
-      </c>
-      <c r="H11" s="30" t="s">
+    <row r="15" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="40"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="64" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J15" s="65" t="s">
+        <v>77</v>
+      </c>
+      <c r="K15" s="66"/>
+      <c r="L15" s="67"/>
+      <c r="M15" s="68"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="42"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="52"/>
+      <c r="E16" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J16" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="K16" s="44"/>
+      <c r="L16" s="45"/>
+      <c r="M16" s="46"/>
+    </row>
+    <row r="17" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="40"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="11"/>
+      <c r="E17" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="K17" s="38"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="39"/>
+    </row>
+    <row r="18" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="40"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="53"/>
+      <c r="E18" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J18" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="K18" s="41"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="39"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="42"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="52"/>
+      <c r="E19" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="J19" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="K19" s="44"/>
+      <c r="L19" s="45"/>
+      <c r="M19" s="46"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="42"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="52"/>
+      <c r="E20" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="I11" s="17" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
-        <v>So That</v>
-      </c>
-      <c r="J11" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="K11" s="39"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="40"/>
+      <c r="I20" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="J20" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="K20" s="44"/>
+      <c r="L20" s="45"/>
+      <c r="M20" s="46"/>
     </row>
-    <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="41">
-        <v>43843</v>
-      </c>
-      <c r="B12" s="56" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="17" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
-        <v>As A</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="17" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
-        <v>I</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="17" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
-        <v>be able to</v>
-      </c>
-      <c r="H12" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="I12" s="17" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
-        <v>So That</v>
-      </c>
-      <c r="J12" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="K12" s="39"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="40"/>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="42"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="52"/>
+      <c r="E21" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="J21" s="63" t="s">
+        <v>55</v>
+      </c>
+      <c r="K21" s="42"/>
+      <c r="L21" s="60"/>
+      <c r="M21" s="61"/>
     </row>
-    <row r="13" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="41">
-        <v>43843</v>
-      </c>
-      <c r="B13" s="56" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="17" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
-        <v>As A</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="17" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
-        <v>I</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="17" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
-        <v>be able to</v>
-      </c>
-      <c r="H13" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="I13" s="17" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
-        <v>So That</v>
-      </c>
-      <c r="J13" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="K13" s="39"/>
-      <c r="L13" s="38"/>
-      <c r="M13" s="40"/>
-    </row>
-    <row r="14" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="41">
-        <v>43843</v>
-      </c>
-      <c r="B14" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="17" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
-        <v>As A</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="17" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
-        <v>I</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G14" s="17" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
-        <v>be able to</v>
-      </c>
-      <c r="H14" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="I14" s="17" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
-        <v>So That</v>
-      </c>
-      <c r="J14" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="K14" s="39"/>
-      <c r="L14" s="38"/>
-      <c r="M14" s="40"/>
-    </row>
-    <row r="15" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="41"/>
-      <c r="B15" s="56"/>
-      <c r="C15" s="17" t="str">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="42"/>
+      <c r="B22" s="56"/>
+      <c r="C22" s="17" t="str">
         <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
         <v/>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="17" t="str">
+      <c r="D22" s="52"/>
+      <c r="E22" s="17" t="str">
         <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
         <v/>
       </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="17" t="str">
+      <c r="F22" s="12"/>
+      <c r="G22" s="17" t="str">
         <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
         <v/>
       </c>
-      <c r="H15" s="65"/>
-      <c r="I15" s="17" t="str">
+      <c r="H22" s="62"/>
+      <c r="I22" s="17" t="str">
         <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
         <v/>
       </c>
-      <c r="J15" s="66"/>
-      <c r="K15" s="67"/>
-      <c r="L15" s="68"/>
-      <c r="M15" s="69"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="43"/>
-      <c r="B16" s="57">
-        <v>2</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G16" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="H16" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="I16" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="J16" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="K16" s="45"/>
-      <c r="L16" s="46"/>
-      <c r="M16" s="47"/>
-    </row>
-    <row r="17" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="41"/>
-      <c r="B17" s="56" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="H17" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="I17" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="J17" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="K17" s="39"/>
-      <c r="L17" s="38"/>
-      <c r="M17" s="40"/>
-    </row>
-    <row r="18" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="41"/>
-      <c r="B18" s="56" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="54" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="H18" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="I18" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="J18" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="K18" s="42"/>
-      <c r="L18" s="38"/>
-      <c r="M18" s="40"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="43"/>
-      <c r="B19" s="57">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="H19" s="49" t="s">
-        <v>64</v>
-      </c>
-      <c r="I19" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="J19" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="K19" s="45"/>
-      <c r="L19" s="46"/>
-      <c r="M19" s="47"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="43"/>
-      <c r="B20" s="57">
-        <v>2.4</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="H20" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="I20" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="J20" s="51" t="s">
-        <v>66</v>
-      </c>
-      <c r="K20" s="45"/>
-      <c r="L20" s="46"/>
-      <c r="M20" s="47"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="43"/>
-      <c r="B21" s="57">
-        <v>2.5</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G21" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="H21" s="63" t="s">
-        <v>68</v>
-      </c>
-      <c r="I21" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="J21" s="64" t="s">
-        <v>69</v>
-      </c>
-      <c r="K21" s="43"/>
-      <c r="L21" s="61"/>
-      <c r="M21" s="62"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="43"/>
-      <c r="B22" s="57"/>
-      <c r="C22" s="18" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
-        <v/>
-      </c>
-      <c r="D22" s="53"/>
-      <c r="E22" s="18" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
-        <v/>
-      </c>
-      <c r="F22" s="12"/>
-      <c r="G22" s="18" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
-        <v/>
-      </c>
-      <c r="H22" s="63"/>
-      <c r="I22" s="18" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
-        <v/>
-      </c>
-      <c r="J22" s="64"/>
-      <c r="K22" s="43"/>
-      <c r="L22" s="61"/>
-      <c r="M22" s="62"/>
+      <c r="J22" s="63"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="60"/>
+      <c r="M22" s="61"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="43"/>
-      <c r="B23" s="44">
-        <v>3</v>
-      </c>
-      <c r="C23" s="18" t="s">
+      <c r="A23" s="42"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" s="18" t="s">
+      <c r="D23" s="12"/>
+      <c r="E23" s="17" t="s">
         <v>24</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G23" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G23" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="H23" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="I23" s="18" t="s">
+      <c r="H23" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="I23" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="J23" s="51" t="s">
-        <v>71</v>
-      </c>
-      <c r="K23" s="45"/>
-      <c r="L23" s="46"/>
-      <c r="M23" s="47"/>
+      <c r="J23" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="K23" s="44"/>
+      <c r="L23" s="45"/>
+      <c r="M23" s="46"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="43"/>
-      <c r="B24" s="44">
-        <v>3.1</v>
-      </c>
-      <c r="C24" s="18" t="s">
+      <c r="A24" s="42"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>67</v>
+      <c r="D24" s="12"/>
+      <c r="E24" s="17" t="s">
+        <v>53</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G24" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="H24" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="I24" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="J24" s="51" t="s">
-        <v>74</v>
-      </c>
-      <c r="K24" s="45"/>
-      <c r="L24" s="46"/>
-      <c r="M24" s="47"/>
+        <v>33</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="H24" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="I24" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="J24" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="K24" s="44"/>
+      <c r="L24" s="45"/>
+      <c r="M24" s="46"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="43"/>
-      <c r="B25" s="44">
-        <v>3.2</v>
-      </c>
-      <c r="C25" s="18" t="s">
+      <c r="A25" s="42"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>67</v>
+      <c r="D25" s="12"/>
+      <c r="E25" s="17" t="s">
+        <v>53</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G25" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="H25" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="I25" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="J25" s="51" t="s">
-        <v>78</v>
-      </c>
-      <c r="K25" s="45"/>
-      <c r="L25" s="46"/>
-      <c r="M25" s="47"/>
+        <v>33</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="H25" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="I25" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="J25" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="K25" s="44"/>
+      <c r="L25" s="45"/>
+      <c r="M25" s="46"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="45"/>
-      <c r="B26" s="13">
-        <v>3.3</v>
-      </c>
-      <c r="C26" s="19" t="s">
+      <c r="A26" s="44"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>67</v>
+      <c r="D26" s="13"/>
+      <c r="E26" s="18" t="s">
+        <v>53</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G26" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="H26" s="50" t="s">
-        <v>79</v>
-      </c>
-      <c r="I26" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="H26" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="I26" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="J26" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="J26" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="K26" s="45"/>
-      <c r="L26" s="46"/>
-      <c r="M26" s="47"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="45"/>
+      <c r="M26" s="46"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="58"/>
-      <c r="B27" s="12">
-        <v>3.4</v>
-      </c>
-      <c r="C27" s="18" t="s">
+      <c r="A27" s="57"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E27" s="18" t="s">
+      <c r="D27" s="12"/>
+      <c r="E27" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="H27" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="I27" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="J27" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="F27" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G27" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="H27" s="59" t="s">
-        <v>81</v>
-      </c>
-      <c r="I27" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="J27" s="60" t="s">
-        <v>82</v>
-      </c>
-      <c r="K27" s="43"/>
-      <c r="L27" s="61"/>
-      <c r="M27" s="62"/>
+      <c r="K27" s="42"/>
+      <c r="L27" s="60"/>
+      <c r="M27" s="61"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="58"/>
+      <c r="A28" s="57"/>
       <c r="B28" s="12"/>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="17" t="s">
         <v>22</v>
       </c>
       <c r="D28" s="12"/>
-      <c r="E28" s="18" t="s">
-        <v>67</v>
+      <c r="E28" s="17" t="s">
+        <v>53</v>
       </c>
       <c r="F28" s="12"/>
-      <c r="G28" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="H28" s="63"/>
-      <c r="I28" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="J28" s="64"/>
-      <c r="K28" s="43"/>
-      <c r="L28" s="61"/>
-      <c r="M28" s="62"/>
+      <c r="G28" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="H28" s="62"/>
+      <c r="I28" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="J28" s="63"/>
+      <c r="K28" s="42"/>
+      <c r="L28" s="60"/>
+      <c r="M28" s="61"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="58"/>
+      <c r="A29" s="57"/>
       <c r="B29" s="12"/>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="17" t="s">
         <v>22</v>
       </c>
       <c r="D29" s="12"/>
-      <c r="E29" s="18" t="s">
-        <v>67</v>
+      <c r="E29" s="17" t="s">
+        <v>53</v>
       </c>
       <c r="F29" s="12"/>
-      <c r="G29" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="H29" s="63"/>
-      <c r="I29" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="J29" s="64"/>
-      <c r="K29" s="43"/>
-      <c r="L29" s="61"/>
-      <c r="M29" s="62"/>
+      <c r="G29" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="H29" s="62"/>
+      <c r="I29" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="J29" s="63"/>
+      <c r="K29" s="42"/>
+      <c r="L29" s="60"/>
+      <c r="M29" s="61"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="58"/>
+      <c r="A30" s="57"/>
       <c r="B30" s="12"/>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="17" t="s">
         <v>22</v>
       </c>
       <c r="D30" s="12"/>
-      <c r="E30" s="18" t="s">
-        <v>67</v>
+      <c r="E30" s="17" t="s">
+        <v>53</v>
       </c>
       <c r="F30" s="12"/>
-      <c r="G30" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="H30" s="63"/>
-      <c r="I30" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="J30" s="64"/>
-      <c r="K30" s="43"/>
-      <c r="L30" s="61"/>
-      <c r="M30" s="62"/>
+      <c r="G30" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="H30" s="62"/>
+      <c r="I30" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="J30" s="63"/>
+      <c r="K30" s="42"/>
+      <c r="L30" s="60"/>
+      <c r="M30" s="61"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="58"/>
+      <c r="A31" s="57"/>
       <c r="B31" s="12"/>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="17" t="s">
         <v>22</v>
       </c>
       <c r="D31" s="12"/>
-      <c r="E31" s="18" t="s">
-        <v>67</v>
+      <c r="E31" s="17" t="s">
+        <v>53</v>
       </c>
       <c r="F31" s="12"/>
-      <c r="G31" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="H31" s="63"/>
-      <c r="I31" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="J31" s="64"/>
-      <c r="K31" s="43"/>
-      <c r="L31" s="61"/>
-      <c r="M31" s="62"/>
+      <c r="G31" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="H31" s="62"/>
+      <c r="I31" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="J31" s="63"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="60"/>
+      <c r="M31" s="61"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B36" s="3" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:K14">
+  <sortState ref="A6:K14">
     <sortCondition ref="A5"/>
   </sortState>
   <mergeCells count="13">
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="A7:J7"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="K5:M5"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:J1"/>
@@ -2879,53 +2759,59 @@
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="L3:M3"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="A7:J7"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="K5:M5"/>
   </mergeCells>
   <conditionalFormatting sqref="F9:G31">
-    <cfRule type="containsText" dxfId="11" priority="16" stopIfTrue="1" operator="containsText" text="Would">
+    <cfRule type="containsText" dxfId="26" priority="16" stopIfTrue="1" operator="containsText" text="Would">
       <formula>NOT(ISERROR(SEARCH("Would",F9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="17" stopIfTrue="1" operator="containsText" text="Wish">
+    <cfRule type="containsText" dxfId="25" priority="17" stopIfTrue="1" operator="containsText" text="Wish">
       <formula>NOT(ISERROR(SEARCH("Wish",F9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="18" stopIfTrue="1" operator="containsText" text="Could">
+    <cfRule type="containsText" dxfId="24" priority="18" stopIfTrue="1" operator="containsText" text="Could">
       <formula>NOT(ISERROR(SEARCH("Could",F9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="19" stopIfTrue="1" operator="containsText" text="Should">
+    <cfRule type="containsText" dxfId="23" priority="19" stopIfTrue="1" operator="containsText" text="Should">
       <formula>NOT(ISERROR(SEARCH("Should",F9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="20" stopIfTrue="1" operator="containsText" text="Must">
+    <cfRule type="containsText" dxfId="22" priority="20" stopIfTrue="1" operator="containsText" text="Must">
       <formula>NOT(ISERROR(SEARCH("Must",F9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9:F31">
-    <cfRule type="cellIs" dxfId="6" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Won't"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28:G31">
-    <cfRule type="containsText" dxfId="5" priority="2" stopIfTrue="1" operator="containsText" text="Would">
+    <cfRule type="containsText" dxfId="20" priority="2" stopIfTrue="1" operator="containsText" text="Would">
       <formula>NOT(ISERROR(SEARCH("Would",F28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" stopIfTrue="1" operator="containsText" text="Wish">
+    <cfRule type="containsText" dxfId="19" priority="3" stopIfTrue="1" operator="containsText" text="Wish">
       <formula>NOT(ISERROR(SEARCH("Wish",F28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="4" stopIfTrue="1" operator="containsText" text="Could">
+    <cfRule type="containsText" dxfId="18" priority="4" stopIfTrue="1" operator="containsText" text="Could">
       <formula>NOT(ISERROR(SEARCH("Could",F28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="5" stopIfTrue="1" operator="containsText" text="Should">
+    <cfRule type="containsText" dxfId="17" priority="5" stopIfTrue="1" operator="containsText" text="Should">
       <formula>NOT(ISERROR(SEARCH("Should",F28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="6" stopIfTrue="1" operator="containsText" text="Must">
+    <cfRule type="containsText" dxfId="16" priority="6" stopIfTrue="1" operator="containsText" text="Must">
       <formula>NOT(ISERROR(SEARCH("Must",F28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28:F31">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Won't"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="J3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" scale="58" fitToHeight="0" orientation="landscape" r:id="rId2"/>
@@ -2945,12 +2831,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005B279478631CDD44835F063507A68C7C" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ab65567a022fb127b02ef4cc56210864">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a02203c3-b4ad-46c2-9cc6-afa11feeea88" xmlns:ns4="aa607228-e39b-4d1c-8048-bb18041aeaf5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2c5a07e74fe33fe960b1997079e11a0e" ns3:_="" ns4:_="">
     <xsd:import namespace="a02203c3-b4ad-46c2-9cc6-afa11feeea88"/>
@@ -3121,6 +3001,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAA5EE75-7E08-4B0E-872A-91BB3A1CEAB7}">
   <ds:schemaRefs>
@@ -3130,15 +3016,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17B40AFA-D9CA-4B45-BF89-8F3FC5E8B4C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5E9EB56-3213-409A-A3D7-6E27657212C4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3155,4 +3032,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17B40AFA-D9CA-4B45-BF89-8F3FC5E8B4C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated orders table to reflect differnt roles and database seeder to insert new data, document update
</commit_message>
<xml_diff>
--- a/Documentation/Information/Feature Analysis-MoSCoW-v17.xlsx
+++ b/Documentation/Information/Feature Analysis-MoSCoW-v17.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20069271\Documents\GitHub\NavyFoodSecurity\Documentation\Information\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHubRepo\NavyFoodSecurity\Documentation\Information\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0F2364B-9769-453C-BEF1-CDAD1259A448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories (MoSCoW)" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'User Stories (MoSCoW)'!$A$8:$K$31</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'User Stories (MoSCoW)'!$A$1:$M$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'User Stories (MoSCoW)'!$A$8:$K$60</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'User Stories (MoSCoW)'!$A$1:$M$20</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'User Stories (MoSCoW)'!$1:$8</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -36,15 +38,12 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="66">
   <si>
     <t>Project:</t>
   </si>
@@ -175,81 +174,21 @@
     <t>when I have lost my password, I can reset it</t>
   </si>
   <si>
-    <t>Browse Users</t>
-  </si>
-  <si>
-    <t>Manage Users</t>
-  </si>
-  <si>
-    <t>I can Manage Users</t>
-  </si>
-  <si>
-    <t>Delete User</t>
-  </si>
-  <si>
-    <t>Unauthorised personnel cannot access the system</t>
-  </si>
-  <si>
-    <t>Edit User</t>
-  </si>
-  <si>
-    <t>Permissons can be changed for users</t>
-  </si>
-  <si>
-    <t>Add User</t>
-  </si>
-  <si>
-    <t xml:space="preserve">So That </t>
-  </si>
-  <si>
-    <t>To view current users in database</t>
-  </si>
-  <si>
     <t xml:space="preserve">I </t>
   </si>
   <si>
     <t>Manage Deliveries</t>
   </si>
   <si>
-    <t>I can manage delivery locations</t>
-  </si>
-  <si>
-    <t>Unauthorised Personnel cannot access sensitive GPS data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">be able to </t>
-  </si>
-  <si>
-    <t>Track Delivery GPS Information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I know where/when deliveries are going to arrive at their destination </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> be able to</t>
-  </si>
-  <si>
     <t>Add Delivery Locations</t>
   </si>
   <si>
-    <t xml:space="preserve">So that </t>
-  </si>
-  <si>
-    <t>Users can see how to get to a destination and how long it may take.</t>
-  </si>
-  <si>
     <t>Browse Deliveries</t>
   </si>
   <si>
-    <t>I can confirm the right person delivered the cargo.</t>
-  </si>
-  <si>
     <t>View contents of a delivery</t>
   </si>
   <si>
-    <t>Users can confirm all contents of a delivery arrived at the destination intact.</t>
-  </si>
-  <si>
     <t>Quick How To:</t>
   </si>
   <si>
@@ -278,12 +217,36 @@
   </si>
   <si>
     <t>An order can be placed</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>change my role</t>
+  </si>
+  <si>
+    <t>I say what I'm doing right now</t>
+  </si>
+  <si>
+    <t>Handle CRUD(Create,Read,Update,Delete) for Users</t>
+  </si>
+  <si>
+    <t>I can create, read, update, delete an entry for a user</t>
+  </si>
+  <si>
+    <t>look at old orders</t>
+  </si>
+  <si>
+    <t>I can see what the has been ordered so far</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -732,7 +695,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -820,9 +783,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -886,9 +846,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -919,9 +876,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" indent="2"/>
     </xf>
@@ -933,6 +887,102 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment indent="8"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment indent="8"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment indent="9"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment indent="9"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment indent="10"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment indent="10"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment indent="11"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment indent="11"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment indent="12"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment indent="12"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment indent="13"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment indent="13"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment indent="14"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment indent="14"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment indent="15"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment indent="15"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1025,7 +1075,7 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="51">
     <dxf>
       <font>
         <strike val="0"/>
@@ -1299,6 +1349,237 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1555,14 +1836,14 @@
       </border>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultTableStyle="NMT Table" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="NMT Table" pivot="0" count="6">
-      <tableStyleElement type="wholeTable" dxfId="32"/>
-      <tableStyleElement type="headerRow" dxfId="31"/>
-      <tableStyleElement type="totalRow" dxfId="30"/>
-      <tableStyleElement type="firstColumn" dxfId="29"/>
-      <tableStyleElement type="firstRowStripe" dxfId="28"/>
-      <tableStyleElement type="secondRowStripe" dxfId="27"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="NMT Table" pivot="0" count="6" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="wholeTable" dxfId="50"/>
+      <tableStyleElement type="headerRow" dxfId="49"/>
+      <tableStyleElement type="totalRow" dxfId="48"/>
+      <tableStyleElement type="firstColumn" dxfId="47"/>
+      <tableStyleElement type="firstRowStripe" dxfId="46"/>
+      <tableStyleElement type="secondRowStripe" dxfId="45"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1577,8 +1858,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:M31" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A8:M31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A8:M60" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A8:M60" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1592,27 +1873,27 @@
     <filterColumn colId="12" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" name="Date Added" dataDxfId="12"/>
-    <tableColumn id="2" name="ID" dataDxfId="11"/>
-    <tableColumn id="3" name="As A" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date Added" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ID" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="As A" dataDxfId="10">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="User Type/Role" dataDxfId="9"/>
-    <tableColumn id="5" name="I" dataDxfId="8">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="User Type/Role" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="I" dataDxfId="8">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="MoSCoW Priority" dataDxfId="7"/>
-    <tableColumn id="7" name="be able to" dataDxfId="6">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="MoSCoW Priority" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="be able to" dataDxfId="6">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Feature Description" dataDxfId="5"/>
-    <tableColumn id="9" name="So That" dataDxfId="4">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Feature Description" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="So That" dataDxfId="4">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Business Reason" dataDxfId="3"/>
-    <tableColumn id="15" name="Version" dataDxfId="2"/>
-    <tableColumn id="14" name="Developer (s) Responsible" dataDxfId="1"/>
-    <tableColumn id="13" name="Acceptance Criteria" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Business Reason" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Version" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Developer (s) Responsible" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Acceptance Criteria" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="NMT Table" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1889,15 +2170,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:M62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="129" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <pane ySplit="8" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1909,48 +2190,48 @@
     <col min="5" max="5" width="5" style="14" customWidth="1"/>
     <col min="6" max="6" width="19.5" style="24" customWidth="1"/>
     <col min="7" max="7" width="14.125" style="24" customWidth="1"/>
-    <col min="8" max="8" width="51.125" style="47" customWidth="1"/>
+    <col min="8" max="8" width="55.625" style="46" customWidth="1"/>
     <col min="9" max="9" width="10.75" style="24" customWidth="1"/>
-    <col min="10" max="10" width="63" style="47" customWidth="1"/>
+    <col min="10" max="10" width="63" style="46" customWidth="1"/>
     <col min="11" max="11" width="11.75" customWidth="1"/>
     <col min="12" max="12" width="30" customWidth="1"/>
     <col min="13" max="13" width="62.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="82" t="s">
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="80" t="s">
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="81"/>
-      <c r="M1" s="84"/>
+      <c r="L1" s="110"/>
+      <c r="M1" s="113"/>
     </row>
     <row r="2" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
       <c r="I2" s="19" t="s">
         <v>5</v>
       </c>
@@ -1960,22 +2241,22 @@
       <c r="K2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="86" t="s">
+      <c r="L2" s="115" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="87"/>
+      <c r="M2" s="116"/>
     </row>
     <row r="3" spans="1:13" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="114"/>
       <c r="G3" s="21" t="s">
         <v>11</v>
       </c>
@@ -1991,53 +2272,53 @@
       <c r="K3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="85" t="s">
+      <c r="L3" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="88"/>
+      <c r="M3" s="117"/>
     </row>
     <row r="4" spans="1:13" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:13" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="75"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="76"/>
-      <c r="L5" s="77"/>
-      <c r="M5" s="78"/>
+      <c r="B5" s="104"/>
+      <c r="C5" s="104"/>
+      <c r="D5" s="104"/>
+      <c r="E5" s="104"/>
+      <c r="F5" s="104"/>
+      <c r="G5" s="103"/>
+      <c r="H5" s="103"/>
+      <c r="I5" s="100"/>
+      <c r="J5" s="100"/>
+      <c r="K5" s="105"/>
+      <c r="L5" s="106"/>
+      <c r="M5" s="107"/>
     </row>
     <row r="6" spans="1:13" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:13" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="69" t="s">
+      <c r="B7" s="102"/>
+      <c r="C7" s="102"/>
+      <c r="D7" s="102"/>
+      <c r="E7" s="102"/>
+      <c r="F7" s="102"/>
+      <c r="G7" s="102"/>
+      <c r="H7" s="102"/>
+      <c r="I7" s="102"/>
+      <c r="J7" s="102"/>
+      <c r="K7" s="98" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="70"/>
+      <c r="L7" s="99"/>
       <c r="M7" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="31" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="15" t="s">
@@ -2067,26 +2348,26 @@
       <c r="J8" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="K8" s="33" t="s">
+      <c r="K8" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="L8" s="34" t="s">
+      <c r="L8" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="M8" s="35" t="s">
+      <c r="M8" s="34" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="36"/>
-      <c r="B9" s="54">
+      <c r="A9" s="35"/>
+      <c r="B9" s="52">
         <v>1</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>24</v>
@@ -2106,18 +2387,18 @@
       <c r="J9" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="K9" s="38"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="39"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="38"/>
     </row>
     <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="40"/>
-      <c r="B10" s="55"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="53"/>
       <c r="C10" s="17" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>24</v>
@@ -2137,18 +2418,18 @@
       <c r="J10" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="K10" s="38"/>
-      <c r="L10" s="37"/>
-      <c r="M10" s="39"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="38"/>
     </row>
     <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="40"/>
-      <c r="B11" s="55"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="53"/>
       <c r="C11" s="17" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>24</v>
@@ -2160,26 +2441,26 @@
         <v>26</v>
       </c>
       <c r="H11" s="29" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="I11" s="17" t="s">
         <v>28</v>
       </c>
       <c r="J11" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="K11" s="38"/>
-      <c r="L11" s="37"/>
-      <c r="M11" s="39"/>
+        <v>54</v>
+      </c>
+      <c r="K11" s="37"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="38"/>
     </row>
     <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="40"/>
-      <c r="B12" s="55"/>
+      <c r="A12" s="39"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="17" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>24</v>
@@ -2199,18 +2480,18 @@
       <c r="J12" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="K12" s="38"/>
-      <c r="L12" s="37"/>
-      <c r="M12" s="39"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="38"/>
     </row>
     <row r="13" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="40"/>
-      <c r="B13" s="55"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="53"/>
       <c r="C13" s="17" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="E13" s="17" t="s">
         <v>24</v>
@@ -2230,18 +2511,18 @@
       <c r="J13" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="K13" s="38"/>
-      <c r="L13" s="37"/>
-      <c r="M13" s="39"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="38"/>
     </row>
     <row r="14" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="40"/>
-      <c r="B14" s="55"/>
+      <c r="A14" s="39"/>
+      <c r="B14" s="53"/>
       <c r="C14" s="17" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="E14" s="17" t="s">
         <v>24</v>
@@ -2253,26 +2534,26 @@
         <v>26</v>
       </c>
       <c r="H14" s="29" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="I14" s="17" t="s">
         <v>28</v>
       </c>
       <c r="J14" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="K14" s="38"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="39"/>
+        <v>52</v>
+      </c>
+      <c r="K14" s="37"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="38"/>
     </row>
     <row r="15" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="40"/>
-      <c r="B15" s="55"/>
+      <c r="A15" s="39"/>
+      <c r="B15" s="53"/>
       <c r="C15" s="17" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="E15" s="17" t="s">
         <v>24</v>
@@ -2283,472 +2564,1259 @@
       <c r="G15" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="64" t="s">
-        <v>76</v>
+      <c r="H15" s="70" t="s">
+        <v>56</v>
       </c>
       <c r="I15" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="65" t="s">
-        <v>77</v>
-      </c>
-      <c r="K15" s="66"/>
-      <c r="L15" s="67"/>
-      <c r="M15" s="68"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="42"/>
-      <c r="B16" s="56"/>
-      <c r="C16" s="17" t="s">
+      <c r="J15" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="K15" s="63"/>
+      <c r="L15" s="64"/>
+      <c r="M15" s="65"/>
+    </row>
+    <row r="16" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="39"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="52"/>
-      <c r="E16" s="17" t="s">
+      <c r="D16" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H16" s="48" t="s">
-        <v>44</v>
+      <c r="H16" s="75" t="s">
+        <v>60</v>
       </c>
       <c r="I16" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="J16" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="K16" s="44"/>
-      <c r="L16" s="45"/>
-      <c r="M16" s="46"/>
-    </row>
-    <row r="17" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="40"/>
-      <c r="B17" s="55"/>
-      <c r="C17" s="16" t="s">
-        <v>22</v>
+      <c r="J16" s="76" t="s">
+        <v>61</v>
+      </c>
+      <c r="K16" s="63"/>
+      <c r="L16" s="64"/>
+      <c r="M16" s="65"/>
+    </row>
+    <row r="17" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="39"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
+        <v/>
       </c>
       <c r="D17" s="11"/>
-      <c r="E17" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="H17" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="I17" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="J17" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="K17" s="38"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="39"/>
-    </row>
-    <row r="18" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="40"/>
-      <c r="B18" s="55"/>
-      <c r="C18" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="53"/>
-      <c r="E18" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="H18" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="I18" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="J18" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="K18" s="41"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="39"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="42"/>
-      <c r="B19" s="56"/>
+      <c r="E17" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
+        <v/>
+      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="69"/>
+      <c r="K17" s="63"/>
+      <c r="L17" s="64"/>
+      <c r="M17" s="65"/>
+    </row>
+    <row r="18" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="39"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
+        <v/>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
+        <v/>
+      </c>
+      <c r="F18" s="11"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="69"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="64"/>
+      <c r="M18" s="65"/>
+    </row>
+    <row r="19" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="39"/>
+      <c r="B19" s="53"/>
       <c r="C19" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="52"/>
+      <c r="D19" s="71" t="s">
+        <v>58</v>
+      </c>
       <c r="E19" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="17" t="s">
+      <c r="G19" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H19" s="48" t="s">
-        <v>50</v>
+      <c r="H19" s="70" t="s">
+        <v>56</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="J19" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="K19" s="44"/>
-      <c r="L19" s="45"/>
-      <c r="M19" s="46"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="42"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J19" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="K19" s="63"/>
+      <c r="L19" s="64"/>
+      <c r="M19" s="65"/>
+    </row>
+    <row r="20" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="39"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="52"/>
-      <c r="E20" s="17" t="s">
+      <c r="D20" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G20" s="17" t="s">
+      <c r="F20" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H20" s="48" t="s">
-        <v>43</v>
+      <c r="H20" s="27" t="s">
+        <v>62</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="J20" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="K20" s="44"/>
-      <c r="L20" s="45"/>
-      <c r="M20" s="46"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="42"/>
-      <c r="B21" s="56"/>
-      <c r="C21" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J20" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="K20" s="37"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="38"/>
+    </row>
+    <row r="21" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="39"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="52"/>
+      <c r="D21" s="71" t="s">
+        <v>58</v>
+      </c>
       <c r="E21" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="10" t="s">
         <v>33</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="H21" s="62" t="s">
-        <v>54</v>
+      <c r="H21" s="27" t="s">
+        <v>34</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="J21" s="63" t="s">
-        <v>55</v>
-      </c>
-      <c r="K21" s="42"/>
-      <c r="L21" s="60"/>
-      <c r="M21" s="61"/>
+        <v>28</v>
+      </c>
+      <c r="J21" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="K21" s="40"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="38"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="42"/>
-      <c r="B22" s="56"/>
-      <c r="C22" s="17" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
-        <v/>
-      </c>
-      <c r="D22" s="52"/>
-      <c r="E22" s="17" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
-        <v/>
-      </c>
-      <c r="F22" s="12"/>
-      <c r="G22" s="17" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
-        <v/>
-      </c>
-      <c r="H22" s="62"/>
-      <c r="I22" s="17" t="str">
-        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
-        <v/>
-      </c>
-      <c r="J22" s="63"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="60"/>
-      <c r="M22" s="61"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="I22" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J22" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="K22" s="43"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="45"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="42"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="17" t="s">
+      <c r="A23" s="41"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="12"/>
+      <c r="D23" s="71" t="s">
+        <v>58</v>
+      </c>
       <c r="E23" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F23" s="10" t="s">
         <v>33</v>
       </c>
       <c r="G23" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="H23" s="48" t="s">
-        <v>54</v>
+      <c r="H23" s="29" t="s">
+        <v>53</v>
       </c>
       <c r="I23" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="J23" s="50" t="s">
+      <c r="J23" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="K23" s="41"/>
+      <c r="L23" s="58"/>
+      <c r="M23" s="59"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="41"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H24" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="I24" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J24" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="K24" s="41"/>
+      <c r="L24" s="58"/>
+      <c r="M24" s="59"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="41"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H25" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="I25" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J25" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="K25" s="41"/>
+      <c r="L25" s="58"/>
+      <c r="M25" s="59"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="41"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="I26" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J26" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="K26" s="41"/>
+      <c r="L26" s="58"/>
+      <c r="M26" s="59"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="41"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H27" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="K23" s="44"/>
-      <c r="L23" s="45"/>
-      <c r="M23" s="46"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="42"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="17" t="s">
+      <c r="I27" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J27" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="K27" s="41"/>
+      <c r="L27" s="58"/>
+      <c r="M27" s="59"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="41"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="12" t="s">
+      <c r="D28" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G24" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="H24" s="48" t="s">
+      <c r="G28" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H28" s="75" t="s">
+        <v>60</v>
+      </c>
+      <c r="I28" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J28" s="76" t="s">
+        <v>61</v>
+      </c>
+      <c r="K28" s="41"/>
+      <c r="L28" s="58"/>
+      <c r="M28" s="59"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="41"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="I24" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="J24" s="50" t="s">
+      <c r="E29" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G29" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H29" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="J29" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="K29" s="43"/>
+      <c r="L29" s="44"/>
+      <c r="M29" s="45"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="41"/>
+      <c r="B30" s="54"/>
+      <c r="C30" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="71"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="77"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="74"/>
+      <c r="K30" s="41"/>
+      <c r="L30" s="58"/>
+      <c r="M30" s="59"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="41"/>
+      <c r="B31" s="54"/>
+      <c r="C31" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="51"/>
+      <c r="E31" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
+        <v/>
+      </c>
+      <c r="F31" s="12"/>
+      <c r="G31" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
+        <v/>
+      </c>
+      <c r="H31" s="66"/>
+      <c r="I31" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
+        <v/>
+      </c>
+      <c r="J31" s="67"/>
+      <c r="K31" s="41"/>
+      <c r="L31" s="58"/>
+      <c r="M31" s="59"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="41"/>
+      <c r="B32" s="54"/>
+      <c r="C32" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="51"/>
+      <c r="E32" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
+        <v/>
+      </c>
+      <c r="F32" s="12"/>
+      <c r="G32" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
+        <v/>
+      </c>
+      <c r="H32" s="66"/>
+      <c r="I32" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
+        <v/>
+      </c>
+      <c r="J32" s="67"/>
+      <c r="K32" s="41"/>
+      <c r="L32" s="58"/>
+      <c r="M32" s="59"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="41"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="51"/>
+      <c r="E33" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
+        <v/>
+      </c>
+      <c r="F33" s="12"/>
+      <c r="G33" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
+        <v/>
+      </c>
+      <c r="H33" s="66"/>
+      <c r="I33" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
+        <v/>
+      </c>
+      <c r="J33" s="67"/>
+      <c r="K33" s="41"/>
+      <c r="L33" s="58"/>
+      <c r="M33" s="59"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="41"/>
+      <c r="B34" s="54"/>
+      <c r="C34" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="51"/>
+      <c r="E34" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
+        <v/>
+      </c>
+      <c r="F34" s="12"/>
+      <c r="G34" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H34" s="66"/>
+      <c r="I34" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J34" s="67"/>
+      <c r="K34" s="41"/>
+      <c r="L34" s="58"/>
+      <c r="M34" s="59"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="41"/>
+      <c r="B35" s="54"/>
+      <c r="C35" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="51"/>
+      <c r="E35" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
+        <v/>
+      </c>
+      <c r="F35" s="12"/>
+      <c r="G35" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H35" s="72"/>
+      <c r="I35" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J35" s="73"/>
+      <c r="K35" s="41"/>
+      <c r="L35" s="58"/>
+      <c r="M35" s="59"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="41"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="51"/>
+      <c r="E36" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
+        <v/>
+      </c>
+      <c r="F36" s="12"/>
+      <c r="G36" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H36" s="60"/>
+      <c r="I36" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J36" s="61"/>
+      <c r="K36" s="41"/>
+      <c r="L36" s="58"/>
+      <c r="M36" s="59"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="41"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="K24" s="44"/>
-      <c r="L24" s="45"/>
-      <c r="M24" s="46"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="42"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="17" t="s">
+      <c r="E37" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G37" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H37" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="I37" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J37" s="49"/>
+      <c r="K37" s="43"/>
+      <c r="L37" s="44"/>
+      <c r="M37" s="45"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="41"/>
+      <c r="B38" s="42"/>
+      <c r="C38" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="12" t="s">
+      <c r="D38" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G25" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="H25" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="I25" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="J25" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="K25" s="44"/>
-      <c r="L25" s="45"/>
-      <c r="M25" s="46"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="44"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="18" t="s">
+      <c r="G38" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H38" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="I38" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J38" s="49"/>
+      <c r="K38" s="43"/>
+      <c r="L38" s="44"/>
+      <c r="M38" s="45"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="43"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="13" t="s">
+      <c r="D39" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="G26" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="H26" s="49" t="s">
-        <v>64</v>
-      </c>
-      <c r="I26" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="J26" s="51" t="s">
-        <v>65</v>
-      </c>
-      <c r="K26" s="44"/>
-      <c r="L26" s="45"/>
-      <c r="M26" s="46"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="57"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="17" t="s">
+      <c r="G39" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H39" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="I39" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J39" s="50"/>
+      <c r="K39" s="43"/>
+      <c r="L39" s="44"/>
+      <c r="M39" s="45"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" s="55"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="12" t="s">
+      <c r="D40" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F40" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G27" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="H27" s="58" t="s">
-        <v>66</v>
-      </c>
-      <c r="I27" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="J27" s="59" t="s">
-        <v>67</v>
-      </c>
-      <c r="K27" s="42"/>
-      <c r="L27" s="60"/>
-      <c r="M27" s="61"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="57"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="17" t="s">
+      <c r="G40" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H40" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="I40" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J40" s="57"/>
+      <c r="K40" s="41"/>
+      <c r="L40" s="58"/>
+      <c r="M40" s="59"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="55"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28" s="12"/>
-      <c r="G28" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="H28" s="62"/>
-      <c r="I28" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="J28" s="63"/>
-      <c r="K28" s="42"/>
-      <c r="L28" s="60"/>
-      <c r="M28" s="61"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="57"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="17" t="s">
+      <c r="D41" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41" s="12"/>
+      <c r="G41" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H41" s="60"/>
+      <c r="I41" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J41" s="61"/>
+      <c r="K41" s="41"/>
+      <c r="L41" s="58"/>
+      <c r="M41" s="59"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" s="55"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" s="12"/>
-      <c r="G29" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="H29" s="62"/>
-      <c r="I29" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="J29" s="63"/>
-      <c r="K29" s="42"/>
-      <c r="L29" s="60"/>
-      <c r="M29" s="61"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="57"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="17" t="s">
+      <c r="D42" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F42" s="12"/>
+      <c r="G42" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H42" s="60"/>
+      <c r="I42" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J42" s="61"/>
+      <c r="K42" s="41"/>
+      <c r="L42" s="58"/>
+      <c r="M42" s="59"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" s="55"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="12"/>
-      <c r="E30" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F30" s="12"/>
-      <c r="G30" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="H30" s="62"/>
-      <c r="I30" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="J30" s="63"/>
-      <c r="K30" s="42"/>
-      <c r="L30" s="60"/>
-      <c r="M30" s="61"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="57"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="17" t="s">
+      <c r="D43" s="12"/>
+      <c r="E43" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F43" s="12"/>
+      <c r="G43" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H43" s="60"/>
+      <c r="I43" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J43" s="61"/>
+      <c r="K43" s="41"/>
+      <c r="L43" s="58"/>
+      <c r="M43" s="59"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" s="55"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="12"/>
-      <c r="E31" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F31" s="12"/>
-      <c r="G31" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="H31" s="62"/>
-      <c r="I31" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="J31" s="63"/>
-      <c r="K31" s="42"/>
-      <c r="L31" s="60"/>
-      <c r="M31" s="61"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B36" s="3" t="s">
-        <v>70</v>
+      <c r="D44" s="12"/>
+      <c r="E44" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F44" s="12"/>
+      <c r="G44" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H44" s="60"/>
+      <c r="I44" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J44" s="61"/>
+      <c r="K44" s="41"/>
+      <c r="L44" s="58"/>
+      <c r="M44" s="59"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" s="41"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
+        <v/>
+      </c>
+      <c r="D45" s="12"/>
+      <c r="E45" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
+        <v/>
+      </c>
+      <c r="F45" s="12"/>
+      <c r="G45" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
+        <v/>
+      </c>
+      <c r="H45" s="56"/>
+      <c r="I45" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
+        <v/>
+      </c>
+      <c r="J45" s="57"/>
+      <c r="K45" s="41"/>
+      <c r="L45" s="58"/>
+      <c r="M45" s="59"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" s="41"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
+        <v/>
+      </c>
+      <c r="D46" s="12"/>
+      <c r="E46" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
+        <v/>
+      </c>
+      <c r="F46" s="12"/>
+      <c r="G46" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
+        <v/>
+      </c>
+      <c r="H46" s="56"/>
+      <c r="I46" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
+        <v/>
+      </c>
+      <c r="J46" s="57"/>
+      <c r="K46" s="41"/>
+      <c r="L46" s="58"/>
+      <c r="M46" s="59"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" s="41"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
+        <v/>
+      </c>
+      <c r="D47" s="12"/>
+      <c r="E47" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
+        <v/>
+      </c>
+      <c r="F47" s="12"/>
+      <c r="G47" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
+        <v/>
+      </c>
+      <c r="H47" s="56"/>
+      <c r="I47" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
+        <v/>
+      </c>
+      <c r="J47" s="57"/>
+      <c r="K47" s="41"/>
+      <c r="L47" s="58"/>
+      <c r="M47" s="59"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" s="41"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
+        <v/>
+      </c>
+      <c r="D48" s="12"/>
+      <c r="E48" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
+        <v/>
+      </c>
+      <c r="F48" s="12"/>
+      <c r="G48" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
+        <v/>
+      </c>
+      <c r="H48" s="60"/>
+      <c r="I48" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
+        <v/>
+      </c>
+      <c r="J48" s="61"/>
+      <c r="K48" s="41"/>
+      <c r="L48" s="58"/>
+      <c r="M48" s="59"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A49" s="41"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
+        <v/>
+      </c>
+      <c r="D49" s="12"/>
+      <c r="E49" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
+        <v/>
+      </c>
+      <c r="F49" s="12"/>
+      <c r="G49" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
+        <v/>
+      </c>
+      <c r="H49" s="66"/>
+      <c r="I49" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
+        <v/>
+      </c>
+      <c r="J49" s="67"/>
+      <c r="K49" s="41"/>
+      <c r="L49" s="58"/>
+      <c r="M49" s="59"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50" s="41"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
+        <v/>
+      </c>
+      <c r="D50" s="12"/>
+      <c r="E50" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
+        <v/>
+      </c>
+      <c r="F50" s="12"/>
+      <c r="G50" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
+        <v/>
+      </c>
+      <c r="H50" s="72"/>
+      <c r="I50" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
+        <v/>
+      </c>
+      <c r="J50" s="73"/>
+      <c r="K50" s="41"/>
+      <c r="L50" s="58"/>
+      <c r="M50" s="59"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A51" s="41"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
+        <v/>
+      </c>
+      <c r="D51" s="12"/>
+      <c r="E51" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
+        <v/>
+      </c>
+      <c r="F51" s="12"/>
+      <c r="G51" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
+        <v/>
+      </c>
+      <c r="H51" s="78"/>
+      <c r="I51" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
+        <v/>
+      </c>
+      <c r="J51" s="79"/>
+      <c r="K51" s="41"/>
+      <c r="L51" s="58"/>
+      <c r="M51" s="59"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A52" s="41"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
+        <v/>
+      </c>
+      <c r="D52" s="12"/>
+      <c r="E52" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
+        <v/>
+      </c>
+      <c r="F52" s="12"/>
+      <c r="G52" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
+        <v/>
+      </c>
+      <c r="H52" s="80"/>
+      <c r="I52" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
+        <v/>
+      </c>
+      <c r="J52" s="81"/>
+      <c r="K52" s="41"/>
+      <c r="L52" s="58"/>
+      <c r="M52" s="59"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A53" s="41"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
+        <v/>
+      </c>
+      <c r="D53" s="12"/>
+      <c r="E53" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
+        <v/>
+      </c>
+      <c r="F53" s="12"/>
+      <c r="G53" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
+        <v/>
+      </c>
+      <c r="H53" s="82"/>
+      <c r="I53" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
+        <v/>
+      </c>
+      <c r="J53" s="83"/>
+      <c r="K53" s="41"/>
+      <c r="L53" s="58"/>
+      <c r="M53" s="59"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A54" s="41"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
+        <v/>
+      </c>
+      <c r="D54" s="12"/>
+      <c r="E54" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
+        <v/>
+      </c>
+      <c r="F54" s="12"/>
+      <c r="G54" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
+        <v/>
+      </c>
+      <c r="H54" s="84"/>
+      <c r="I54" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
+        <v/>
+      </c>
+      <c r="J54" s="85"/>
+      <c r="K54" s="41"/>
+      <c r="L54" s="58"/>
+      <c r="M54" s="59"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A55" s="41"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
+        <v/>
+      </c>
+      <c r="D55" s="12"/>
+      <c r="E55" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
+        <v/>
+      </c>
+      <c r="F55" s="12"/>
+      <c r="G55" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
+        <v/>
+      </c>
+      <c r="H55" s="86"/>
+      <c r="I55" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
+        <v/>
+      </c>
+      <c r="J55" s="87"/>
+      <c r="K55" s="41"/>
+      <c r="L55" s="58"/>
+      <c r="M55" s="59"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A56" s="41"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
+        <v/>
+      </c>
+      <c r="D56" s="12"/>
+      <c r="E56" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
+        <v/>
+      </c>
+      <c r="F56" s="12"/>
+      <c r="G56" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
+        <v/>
+      </c>
+      <c r="H56" s="88"/>
+      <c r="I56" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
+        <v/>
+      </c>
+      <c r="J56" s="89"/>
+      <c r="K56" s="41"/>
+      <c r="L56" s="58"/>
+      <c r="M56" s="59"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A57" s="41"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
+        <v/>
+      </c>
+      <c r="D57" s="12"/>
+      <c r="E57" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
+        <v/>
+      </c>
+      <c r="F57" s="12"/>
+      <c r="G57" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
+        <v/>
+      </c>
+      <c r="H57" s="90"/>
+      <c r="I57" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
+        <v/>
+      </c>
+      <c r="J57" s="91"/>
+      <c r="K57" s="41"/>
+      <c r="L57" s="58"/>
+      <c r="M57" s="59"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A58" s="41"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
+        <v/>
+      </c>
+      <c r="D58" s="12"/>
+      <c r="E58" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
+        <v/>
+      </c>
+      <c r="F58" s="12"/>
+      <c r="G58" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
+        <v/>
+      </c>
+      <c r="H58" s="92"/>
+      <c r="I58" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
+        <v/>
+      </c>
+      <c r="J58" s="93"/>
+      <c r="K58" s="41"/>
+      <c r="L58" s="58"/>
+      <c r="M58" s="59"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A59" s="41"/>
+      <c r="B59" s="12"/>
+      <c r="C59" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
+        <v/>
+      </c>
+      <c r="D59" s="12"/>
+      <c r="E59" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
+        <v/>
+      </c>
+      <c r="F59" s="12"/>
+      <c r="G59" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
+        <v/>
+      </c>
+      <c r="H59" s="94"/>
+      <c r="I59" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
+        <v/>
+      </c>
+      <c r="J59" s="95"/>
+      <c r="K59" s="41"/>
+      <c r="L59" s="58"/>
+      <c r="M59" s="59"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A60" s="41"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[As A]],"")</f>
+        <v/>
+      </c>
+      <c r="D60" s="12"/>
+      <c r="E60" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[I]],"")</f>
+        <v/>
+      </c>
+      <c r="F60" s="12"/>
+      <c r="G60" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[be able to]],"")</f>
+        <v/>
+      </c>
+      <c r="H60" s="96"/>
+      <c r="I60" s="17" t="str">
+        <f>IF(Table1[[#This Row],[Date Added]]&lt;&gt;"",Table1[[#Headers],[So That]],"")</f>
+        <v/>
+      </c>
+      <c r="J60" s="97"/>
+      <c r="K60" s="41"/>
+      <c r="L60" s="58"/>
+      <c r="M60" s="59"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B62" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A6:K14">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:K14">
     <sortCondition ref="A5"/>
   </sortState>
   <mergeCells count="13">
@@ -2766,52 +3834,118 @@
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="K5:M5"/>
   </mergeCells>
-  <conditionalFormatting sqref="F9:G31">
-    <cfRule type="containsText" dxfId="26" priority="16" stopIfTrue="1" operator="containsText" text="Would">
+  <conditionalFormatting sqref="F9:G16 F17:F18 F20 G17:G20 F29:G44">
+    <cfRule type="containsText" dxfId="44" priority="34" stopIfTrue="1" operator="containsText" text="Would">
       <formula>NOT(ISERROR(SEARCH("Would",F9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="17" stopIfTrue="1" operator="containsText" text="Wish">
+    <cfRule type="containsText" dxfId="43" priority="35" stopIfTrue="1" operator="containsText" text="Wish">
       <formula>NOT(ISERROR(SEARCH("Wish",F9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="18" stopIfTrue="1" operator="containsText" text="Could">
+    <cfRule type="containsText" dxfId="42" priority="36" stopIfTrue="1" operator="containsText" text="Could">
       <formula>NOT(ISERROR(SEARCH("Could",F9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="19" stopIfTrue="1" operator="containsText" text="Should">
+    <cfRule type="containsText" dxfId="41" priority="37" stopIfTrue="1" operator="containsText" text="Should">
       <formula>NOT(ISERROR(SEARCH("Should",F9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="20" stopIfTrue="1" operator="containsText" text="Must">
+    <cfRule type="containsText" dxfId="40" priority="38" stopIfTrue="1" operator="containsText" text="Must">
       <formula>NOT(ISERROR(SEARCH("Must",F9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F9:F31">
-    <cfRule type="cellIs" dxfId="21" priority="14" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="F9:F18 F20 F29:F44">
+    <cfRule type="cellIs" dxfId="39" priority="32" stopIfTrue="1" operator="equal">
       <formula>"Won't"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F28:G31">
+  <conditionalFormatting sqref="F41:F44">
+    <cfRule type="containsText" dxfId="38" priority="20" stopIfTrue="1" operator="containsText" text="Would">
+      <formula>NOT(ISERROR(SEARCH("Would",F41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="21" stopIfTrue="1" operator="containsText" text="Wish">
+      <formula>NOT(ISERROR(SEARCH("Wish",F41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="22" stopIfTrue="1" operator="containsText" text="Could">
+      <formula>NOT(ISERROR(SEARCH("Could",F41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="35" priority="23" stopIfTrue="1" operator="containsText" text="Should">
+      <formula>NOT(ISERROR(SEARCH("Should",F41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="24" stopIfTrue="1" operator="containsText" text="Must">
+      <formula>NOT(ISERROR(SEARCH("Must",F41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F41:F44">
+    <cfRule type="cellIs" dxfId="33" priority="19" stopIfTrue="1" operator="equal">
+      <formula>"Won't"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F19">
+    <cfRule type="containsText" dxfId="32" priority="14" stopIfTrue="1" operator="containsText" text="Would">
+      <formula>NOT(ISERROR(SEARCH("Would",F19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="15" stopIfTrue="1" operator="containsText" text="Wish">
+      <formula>NOT(ISERROR(SEARCH("Wish",F19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="16" stopIfTrue="1" operator="containsText" text="Could">
+      <formula>NOT(ISERROR(SEARCH("Could",F19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="17" stopIfTrue="1" operator="containsText" text="Should">
+      <formula>NOT(ISERROR(SEARCH("Should",F19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="18" stopIfTrue="1" operator="containsText" text="Must">
+      <formula>NOT(ISERROR(SEARCH("Must",F19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F19">
+    <cfRule type="cellIs" dxfId="27" priority="13" stopIfTrue="1" operator="equal">
+      <formula>"Won't"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21:F22">
+    <cfRule type="cellIs" dxfId="26" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Won't"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21:G22">
+    <cfRule type="containsText" dxfId="25" priority="8" stopIfTrue="1" operator="containsText" text="Would">
+      <formula>NOT(ISERROR(SEARCH("Would",F21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="9" stopIfTrue="1" operator="containsText" text="Wish">
+      <formula>NOT(ISERROR(SEARCH("Wish",F21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="23" priority="10" stopIfTrue="1" operator="containsText" text="Could">
+      <formula>NOT(ISERROR(SEARCH("Could",F21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="11" stopIfTrue="1" operator="containsText" text="Should">
+      <formula>NOT(ISERROR(SEARCH("Should",F21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="12" stopIfTrue="1" operator="containsText" text="Must">
+      <formula>NOT(ISERROR(SEARCH("Must",F21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F23:G28">
     <cfRule type="containsText" dxfId="20" priority="2" stopIfTrue="1" operator="containsText" text="Would">
-      <formula>NOT(ISERROR(SEARCH("Would",F28)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Would",F23)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="19" priority="3" stopIfTrue="1" operator="containsText" text="Wish">
-      <formula>NOT(ISERROR(SEARCH("Wish",F28)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Wish",F23)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="18" priority="4" stopIfTrue="1" operator="containsText" text="Could">
-      <formula>NOT(ISERROR(SEARCH("Could",F28)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Could",F23)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="17" priority="5" stopIfTrue="1" operator="containsText" text="Should">
-      <formula>NOT(ISERROR(SEARCH("Should",F28)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Should",F23)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="16" priority="6" stopIfTrue="1" operator="containsText" text="Must">
-      <formula>NOT(ISERROR(SEARCH("Must",F28)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Must",F23)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F28:F31">
+  <conditionalFormatting sqref="F23:F28">
     <cfRule type="cellIs" dxfId="15" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Won't"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J3" r:id="rId1"/>
+    <hyperlink ref="J3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" scale="58" fitToHeight="0" orientation="landscape" r:id="rId2"/>
@@ -2822,15 +3956,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005B279478631CDD44835F063507A68C7C" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ab65567a022fb127b02ef4cc56210864">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a02203c3-b4ad-46c2-9cc6-afa11feeea88" xmlns:ns4="aa607228-e39b-4d1c-8048-bb18041aeaf5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2c5a07e74fe33fe960b1997079e11a0e" ns3:_="" ns4:_="">
     <xsd:import namespace="a02203c3-b4ad-46c2-9cc6-afa11feeea88"/>
@@ -3001,21 +4126,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAA5EE75-7E08-4B0E-872A-91BB3A1CEAB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5E9EB56-3213-409A-A3D7-6E27657212C4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3034,11 +4160,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17B40AFA-D9CA-4B45-BF89-8F3FC5E8B4C0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAA5EE75-7E08-4B0E-872A-91BB3A1CEAB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>